<commit_message>
Change frame design + Trasmitter CodeV1
</commit_message>
<xml_diff>
--- a/ProtocolAndFM/FrameDesign.xlsx
+++ b/ProtocolAndFM/FrameDesign.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Predator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Predator\Desktop\Learning Resources\DataCom\DATA_COMMUNICATIONS_Final_Project\ProtocolAndFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CCCFF5-6481-4CFD-953D-A893642F315A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A435305-FB3A-44D9-8C09-05E44B822882}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4095" windowWidth="28800" windowHeight="11505" xr2:uid="{AD8B754B-3500-4050-A5B7-118D6C963137}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AD8B754B-3500-4050-A5B7-118D6C963137}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>dst 8 bits</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>openFlag 4 bits</t>
+  </si>
+  <si>
+    <t>src 8 bits</t>
   </si>
 </sst>
 </file>
@@ -428,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7C19B84-44D6-4ABD-BB38-3D149610CFB4}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -442,9 +445,10 @@
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="11.375" customWidth="1"/>
     <col min="6" max="6" width="14.25" customWidth="1"/>
+    <col min="7" max="7" width="12.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -452,32 +456,35 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1011</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Change Frame Design again
</commit_message>
<xml_diff>
--- a/ProtocolAndFM/FrameDesign.xlsx
+++ b/ProtocolAndFM/FrameDesign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Predator\Desktop\Learning Resources\DataCom\DATA_COMMUNICATIONS_Final_Project\ProtocolAndFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD97976F-1A09-4F1A-83BB-84EC5137322A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83A7A94-3A8A-42F6-9D03-FE2619BB2F96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1950" windowWidth="28800" windowHeight="11505" xr2:uid="{AD8B754B-3500-4050-A5B7-118D6C963137}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>frameNo 1 bit</t>
   </si>
   <si>
-    <t>data 10 bits</t>
-  </si>
-  <si>
     <t>parity 1 bit</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>char end 0 end</t>
+  </si>
+  <si>
+    <t>data 16 bits</t>
   </si>
 </sst>
 </file>
@@ -440,7 +440,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="G4" sqref="G3:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -457,103 +457,103 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Better frame representation and CRC test
</commit_message>
<xml_diff>
--- a/ProtocolAndFM/FrameDesign.xlsx
+++ b/ProtocolAndFM/FrameDesign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Predator\Desktop\Learning Resources\DataCom\DATA_COMMUNICATIONS_Final_Project\ProtocolAndFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FE9F7B-B76D-4827-96A8-8B86F499211B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990962B5-6B21-4321-AD45-777BB4EA2A8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AD8B754B-3500-4050-A5B7-118D6C963137}"/>
   </bookViews>
@@ -36,37 +36,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
   <si>
-    <t>dst 8 bits</t>
-  </si>
-  <si>
     <t>stop and wait arq</t>
   </si>
   <si>
-    <t>src 8 bits</t>
-  </si>
-  <si>
-    <t>openFlag 8 bits</t>
-  </si>
-  <si>
     <t>char</t>
   </si>
   <si>
-    <t>endFlag 8 bit</t>
-  </si>
-  <si>
     <t>char end 1 more</t>
   </si>
   <si>
     <t>char end 0 end</t>
   </si>
   <si>
-    <t>data 16 bits</t>
-  </si>
-  <si>
     <t>frameNo 1 byte</t>
   </si>
   <si>
-    <t>parity 1 byte</t>
+    <t>data 2 bytes</t>
+  </si>
+  <si>
+    <t>check 1 byte</t>
+  </si>
+  <si>
+    <t>endFlag 1 byte</t>
+  </si>
+  <si>
+    <t>src 1 byte</t>
+  </si>
+  <si>
+    <t>dst 1 byte</t>
+  </si>
+  <si>
+    <t>openFlag 1 byte</t>
   </si>
 </sst>
 </file>
@@ -434,123 +434,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7C19B84-44D6-4ABD-BB38-3D149610CFB4}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="B5:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.875" customWidth="1"/>
-    <col min="2" max="2" width="9.75" customWidth="1"/>
-    <col min="3" max="3" width="15.375" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="11.375" customWidth="1"/>
-    <col min="6" max="6" width="14.25" customWidth="1"/>
-    <col min="7" max="7" width="15.625" customWidth="1"/>
-    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="15.375" customWidth="1"/>
+    <col min="3" max="3" width="11.625" customWidth="1"/>
+    <col min="4" max="4" width="10.625" customWidth="1"/>
+    <col min="5" max="5" width="16.875" customWidth="1"/>
+    <col min="6" max="7" width="13.125" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>